<commit_message>
updating data in home
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538300\Documents\691\gdp_group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA9F014-61D4-4F0A-AF9E-EDA3162DEA25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E47F4F0-ADCB-4534-A3F6-6F0024234B8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{090C377B-AC9E-4432-9958-B414BFE4C8F2}"/>
   </bookViews>
@@ -1140,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6693E31F-BCD6-420F-922C-DA10A299A0A9}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1184,29 +1184,127 @@
       <c r="A3">
         <v>12000</v>
       </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>1800</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>15000</v>
       </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>110</v>
+      </c>
+      <c r="D4">
+        <v>2200</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>20000</v>
       </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+      <c r="D5">
+        <v>2000</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>13000</v>
       </c>
-      <c r="B6"/>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>1900</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>14000</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>130</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>15000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>120</v>
+      </c>
+      <c r="D8">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>21000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>120</v>
+      </c>
+      <c r="D9">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>18000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>110</v>
+      </c>
+      <c r="D10">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>15000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>120</v>
+      </c>
+      <c r="D11">
+        <v>3000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new input for steps
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538300\Documents\691\gdp_group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1373F1-118E-425D-911F-E693DD1F7BD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D268A4F1-B15A-4365-AED3-EA7CED8BBA49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{090C377B-AC9E-4432-9958-B414BFE4C8F2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="4" xr2:uid="{090C377B-AC9E-4432-9958-B414BFE4C8F2}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -1171,7 +1171,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1343,7 +1343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E13748-5FDC-4048-B23E-CD995DA1C665}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -1481,10 +1481,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94D898A-9782-46DE-A19A-69C6D87BB6B2}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1506,7 +1506,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>7000</v>
+        <v>10000</v>
       </c>
       <c r="B2" s="1">
         <v>10000</v>
@@ -1515,12 +1515,104 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>12000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>12000</v>
+      </c>
+      <c r="C3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>15000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>20000</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>20000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>20000</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B6"/>
+      <c r="A6">
+        <v>13000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C6">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="1">
+        <v>14000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>15000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>21000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>20000</v>
+      </c>
+      <c r="C9">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>18000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>20000</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>15000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
inserting data in hydration level
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538300\Documents\691\gdp_group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B4789E-2798-466C-B09F-DE9C6B5C2753}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A100A0E-2ED3-4DF9-8B3A-1D9FDDCB3AEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="5" xr2:uid="{090C377B-AC9E-4432-9958-B414BFE4C8F2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="6" xr2:uid="{090C377B-AC9E-4432-9958-B414BFE4C8F2}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -1171,7 +1171,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1624,7 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FABE246-EA76-4450-9732-8B6AAB9304F6}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1730,15 +1730,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5C73E4-F5F1-43AF-8CF5-DAD34D594BD5}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1751,10 +1751,82 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="1">
+        <v>120</v>
+      </c>
+      <c r="B2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>100</v>
       </c>
-      <c r="B2">
+      <c r="B3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>110</v>
+      </c>
+      <c r="B4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>90</v>
+      </c>
+      <c r="B5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="B6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>130</v>
+      </c>
+      <c r="B7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>120</v>
+      </c>
+      <c r="B8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>120</v>
+      </c>
+      <c r="B9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>110</v>
+      </c>
+      <c r="B10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>120</v>
+      </c>
+      <c r="B11">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating data in Calories
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538300\Documents\691\gdp_group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A100A0E-2ED3-4DF9-8B3A-1D9FDDCB3AEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C31057-7892-461A-B16E-2204B11BF076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="6" xr2:uid="{090C377B-AC9E-4432-9958-B414BFE4C8F2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="7" xr2:uid="{090C377B-AC9E-4432-9958-B414BFE4C8F2}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="89">
   <si>
     <t>user_id</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>calories_goal</t>
-  </si>
-  <si>
-    <t>required_intake</t>
   </si>
   <si>
     <t>alexathegrt@gmail.com</t>
@@ -721,19 +718,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F2" s="1">
         <v>58</v>
@@ -747,19 +744,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3">
         <v>20</v>
@@ -773,19 +770,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4">
         <v>22</v>
@@ -799,19 +796,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5">
         <v>28</v>
@@ -825,19 +822,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -851,19 +848,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7">
         <v>42</v>
@@ -877,19 +874,19 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8">
         <v>99</v>
@@ -903,19 +900,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -929,19 +926,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10">
         <v>40</v>
@@ -955,19 +952,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
         <v>57</v>
-      </c>
-      <c r="E11" t="s">
-        <v>58</v>
       </c>
       <c r="F11">
         <v>38</v>
@@ -1046,16 +1043,16 @@
         <v>1001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1063,16 +1060,16 @@
         <v>1002</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1080,16 +1077,16 @@
         <v>1003</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1097,16 +1094,16 @@
         <v>1004</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1114,16 +1111,16 @@
         <v>1005</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1131,16 +1128,16 @@
         <v>1006</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
         <v>76</v>
-      </c>
-      <c r="E7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1171,13 +1168,14 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.54296875" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1375,7 +1373,7 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G1" t="s">
         <v>8</v>
@@ -1386,10 +1384,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C2" s="3">
         <v>43831</v>
@@ -1401,21 +1399,21 @@
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="1">
         <v>1001</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="4">
         <v>44066</v>
@@ -1427,21 +1425,21 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3">
         <v>1001</v>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="4">
         <v>44066</v>
@@ -1453,13 +1451,13 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4">
         <v>1001</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1732,7 +1730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5C73E4-F5F1-43AF-8CF5-DAD34D594BD5}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1747,7 +1745,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1837,10 +1835,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD78A46-777D-46C0-8477-D558DF0BBFAB}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1851,26 +1849,92 @@
     <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>2500</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>2000</v>
       </c>
       <c r="B2">
         <v>2000</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1800</v>
+      </c>
+      <c r="B3">
         <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2200</v>
+      </c>
+      <c r="B4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2000</v>
+      </c>
+      <c r="B5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1900</v>
+      </c>
+      <c r="B6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B7">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2500</v>
+      </c>
+      <c r="B8">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2300</v>
+      </c>
+      <c r="B9">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2200</v>
+      </c>
+      <c r="B10">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>3000</v>
+      </c>
+      <c r="B11">
+        <v>2500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the user information
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538300\Documents\691\gdp_group4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538343\Documents\691\44691-Module1-Badami4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C31057-7892-461A-B16E-2204B11BF076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DF9A76-7175-4643-B0E6-5FBD2ACB902E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="7" xr2:uid="{090C377B-AC9E-4432-9958-B414BFE4C8F2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{090C377B-AC9E-4432-9958-B414BFE4C8F2}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
     <sheet name="Admin info" sheetId="2" r:id="rId2"/>
-    <sheet name="Home" sheetId="8" r:id="rId3"/>
-    <sheet name="Challenge" sheetId="3" r:id="rId4"/>
+    <sheet name="Challenge" sheetId="3" r:id="rId3"/>
+    <sheet name="Home" sheetId="8" r:id="rId4"/>
     <sheet name="Steps" sheetId="4" r:id="rId5"/>
     <sheet name="Sleep" sheetId="5" r:id="rId6"/>
     <sheet name="Hydration Level" sheetId="6" r:id="rId7"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="122">
   <si>
     <t>user_id</t>
   </si>
@@ -114,12 +114,6 @@
     <t>alexathegrt@gmail.com</t>
   </si>
   <si>
-    <t>Alekhya</t>
-  </si>
-  <si>
-    <t>Jaddu</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
@@ -198,12 +192,6 @@
     <t>arto</t>
   </si>
   <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>sara</t>
-  </si>
-  <si>
     <t>barnes</t>
   </si>
   <si>
@@ -307,6 +295,117 @@
   </si>
   <si>
     <t>barpee hundred</t>
+  </si>
+  <si>
+    <t>neil</t>
+  </si>
+  <si>
+    <t>nmelendz@gmail.com</t>
+  </si>
+  <si>
+    <t>melendz</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Parrish</t>
+  </si>
+  <si>
+    <t>ruth</t>
+  </si>
+  <si>
+    <t>williams</t>
+  </si>
+  <si>
+    <t>claire</t>
+  </si>
+  <si>
+    <t>shawn</t>
+  </si>
+  <si>
+    <t>murphy</t>
+  </si>
+  <si>
+    <t>morgan</t>
+  </si>
+  <si>
+    <t>ryan</t>
+  </si>
+  <si>
+    <t>booth</t>
+  </si>
+  <si>
+    <t>ria</t>
+  </si>
+  <si>
+    <t>jensen</t>
+  </si>
+  <si>
+    <t>hope</t>
+  </si>
+  <si>
+    <t>james</t>
+  </si>
+  <si>
+    <t>pete</t>
+  </si>
+  <si>
+    <t>messer</t>
+  </si>
+  <si>
+    <t>spencer</t>
+  </si>
+  <si>
+    <t>waldorf</t>
+  </si>
+  <si>
+    <t>celine</t>
+  </si>
+  <si>
+    <t>cm1620@gmail.com</t>
+  </si>
+  <si>
+    <t>shawn1597@gmail.com</t>
+  </si>
+  <si>
+    <t>ryanb145@gmail.com</t>
+  </si>
+  <si>
+    <t>littlej@gmail.com</t>
+  </si>
+  <si>
+    <t>lovely.hope@gmail.com</t>
+  </si>
+  <si>
+    <t>petemesser@gmail.com</t>
+  </si>
+  <si>
+    <t>cece153@gmail.com</t>
+  </si>
+  <si>
+    <t>tony26@gmail.com</t>
+  </si>
+  <si>
+    <t>clara</t>
+  </si>
+  <si>
+    <t>murp13</t>
+  </si>
+  <si>
+    <t>rb145</t>
+  </si>
+  <si>
+    <t>shine</t>
+  </si>
+  <si>
+    <t>lovely</t>
+  </si>
+  <si>
+    <t>mustang</t>
+  </si>
+  <si>
+    <t>cece</t>
   </si>
 </sst>
 </file>
@@ -351,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,6 +462,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -678,16 +784,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9072E92-96AB-4278-9757-75DAEE2DBEE6}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -718,45 +826,45 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="5">
         <v>24</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1">
-        <v>58</v>
-      </c>
-      <c r="G2" s="1">
-        <v>50</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="G2" s="5">
+        <v>140</v>
+      </c>
+      <c r="H2" s="5">
         <v>6.2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3">
         <v>20</v>
@@ -770,19 +878,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F4">
         <v>22</v>
@@ -796,19 +904,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F5">
         <v>28</v>
@@ -822,19 +930,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" t="s">
         <v>53</v>
-      </c>
-      <c r="E6" t="s">
-        <v>57</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -848,19 +956,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F7">
         <v>42</v>
@@ -874,22 +982,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="G8">
         <v>185</v>
@@ -900,22 +1008,22 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="G9">
         <v>170</v>
@@ -926,19 +1034,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F10">
         <v>40</v>
@@ -952,19 +1060,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F11">
         <v>38</v>
@@ -976,17 +1084,239 @@
         <v>5.8</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12">
+        <v>45</v>
+      </c>
+      <c r="G12">
+        <v>158</v>
+      </c>
+      <c r="H12">
+        <v>6.4</v>
+      </c>
+    </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13"/>
+      <c r="A13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13">
+        <v>33</v>
+      </c>
+      <c r="G13">
+        <v>138</v>
+      </c>
+      <c r="H13">
+        <v>5.0999999999999996</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="1">
+        <v>27</v>
+      </c>
+      <c r="G14" s="1">
+        <v>159</v>
+      </c>
+      <c r="H14" s="1">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15">
+        <v>41</v>
+      </c>
+      <c r="G15">
+        <v>169</v>
+      </c>
+      <c r="H15">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16">
+        <v>17</v>
+      </c>
+      <c r="G16">
+        <v>130</v>
+      </c>
+      <c r="H16">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17">
+        <v>22</v>
+      </c>
+      <c r="G17">
+        <v>141</v>
+      </c>
+      <c r="H17">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18">
+        <v>43</v>
+      </c>
+      <c r="G18">
+        <v>176</v>
+      </c>
+      <c r="H18">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+      <c r="G19">
+        <v>110</v>
+      </c>
+      <c r="H19">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20">
+        <v>23</v>
+      </c>
+      <c r="G20">
+        <v>159</v>
+      </c>
+      <c r="H20">
+        <v>5.4</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1000,6 +1330,15 @@
     <hyperlink ref="B9" r:id="rId8" xr:uid="{B15E9D71-3D14-48F0-8523-F23939F2D035}"/>
     <hyperlink ref="B10" r:id="rId9" xr:uid="{E750D6A7-2DF3-4D09-985A-5C5E9FEE3A79}"/>
     <hyperlink ref="B11" r:id="rId10" xr:uid="{AFC6F657-DB11-47D8-A3CB-75B6FFD48D82}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{2FF7FAD2-71F6-48C4-B662-D1C463306465}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{EBB34734-DFB2-4A06-AE9F-EC2EA65283C0}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{07FFF31E-8A01-41CD-AF25-8EF820FA537F}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{E424B264-E343-4A5B-9675-50A0041F18F4}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{D5885A5D-EB7A-4EB4-86D5-F43FD6B5082F}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{7D90C5CA-3279-405E-82C7-B96C5A805877}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{E0950F1E-D118-487D-863C-89CE5BE8ADBB}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{FB2E8795-E758-4686-AFE9-04459604D127}"/>
+    <hyperlink ref="B19" r:id="rId19" xr:uid="{72FAC8FC-FB9C-4A0C-92E2-B3DA7E499C80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1043,16 +1382,16 @@
         <v>1001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1060,16 +1399,16 @@
         <v>1002</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1077,16 +1416,16 @@
         <v>1003</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
         <v>72</v>
-      </c>
-      <c r="E4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1094,16 +1433,16 @@
         <v>1004</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
         <v>73</v>
-      </c>
-      <c r="E5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1111,16 +1450,16 @@
         <v>1005</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1128,16 +1467,16 @@
         <v>1006</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1164,184 +1503,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6693E31F-BCD6-420F-922C-DA10A299A0A9}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="15.54296875" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>10000</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1">
-        <v>120</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>12000</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>15000</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>110</v>
-      </c>
-      <c r="D4">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>20000</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>90</v>
-      </c>
-      <c r="D5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>13000</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-      <c r="D6">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>14000</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>130</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>15000</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>120</v>
-      </c>
-      <c r="D8">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>21000</v>
-      </c>
-      <c r="B9" s="1">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>120</v>
-      </c>
-      <c r="D9">
-        <v>2300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>18000</v>
-      </c>
-      <c r="B10" s="1">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>110</v>
-      </c>
-      <c r="D10">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>15000</v>
-      </c>
-      <c r="B11" s="1">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>120</v>
-      </c>
-      <c r="D11">
-        <v>3000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E13748-5FDC-4048-B23E-CD995DA1C665}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -1373,7 +1538,7 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G1" t="s">
         <v>8</v>
@@ -1384,10 +1549,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3">
         <v>43831</v>
@@ -1399,21 +1564,21 @@
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1">
         <v>1001</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4">
         <v>44066</v>
@@ -1425,21 +1590,21 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G3">
         <v>1001</v>
       </c>
       <c r="H3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="4">
         <v>44066</v>
@@ -1451,13 +1616,13 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G4">
         <v>1001</v>
       </c>
       <c r="H4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1477,12 +1642,186 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6693E31F-BCD6-420F-922C-DA10A299A0A9}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>120</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>12000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>15000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>110</v>
+      </c>
+      <c r="D4">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>20000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+      <c r="D5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>13000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>14000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>130</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>15000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>120</v>
+      </c>
+      <c r="D8">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>21000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>120</v>
+      </c>
+      <c r="D9">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>18000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>110</v>
+      </c>
+      <c r="D10">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>15000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>120</v>
+      </c>
+      <c r="D11">
+        <v>3000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94D898A-9782-46DE-A19A-69C6D87BB6B2}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1503,14 +1842,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="A2" s="5">
         <v>10000</v>
       </c>
       <c r="B2" s="1">
         <v>10000</v>
       </c>
-      <c r="C2" s="1">
-        <v>2</v>
+      <c r="C2" s="5">
+        <v>4.3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1532,7 +1871,7 @@
         <v>20000</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1543,7 +1882,7 @@
         <v>20000</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1558,14 +1897,14 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+      <c r="A7" s="5">
         <v>14000</v>
       </c>
       <c r="B7" s="1">
         <v>15000</v>
       </c>
-      <c r="C7" s="1">
-        <v>3</v>
+      <c r="C7" s="5">
+        <v>6.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1576,18 +1915,18 @@
         <v>15000</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>21000</v>
+        <v>17000</v>
       </c>
       <c r="B9" s="1">
-        <v>20000</v>
+        <v>18000</v>
       </c>
       <c r="C9">
-        <v>3.5</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1598,7 +1937,7 @@
         <v>20000</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1609,7 +1948,106 @@
         <v>15000</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>18000</v>
+      </c>
+      <c r="C12">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>17000</v>
+      </c>
+      <c r="C13">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>9000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C14">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>8000</v>
+      </c>
+      <c r="B15" s="1">
+        <v>12000</v>
+      </c>
+      <c r="C15">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>8000</v>
+      </c>
+      <c r="B16" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C16">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>7000</v>
+      </c>
+      <c r="B17" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>7000</v>
+      </c>
+      <c r="B18" s="1">
+        <v>14000</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>4000</v>
+      </c>
+      <c r="B19" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C19">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>6000</v>
+      </c>
+      <c r="B20" s="1">
+        <v>11000</v>
+      </c>
+      <c r="C20">
+        <v>2.6</v>
       </c>
     </row>
   </sheetData>
@@ -1620,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FABE246-EA76-4450-9732-8B6AAB9304F6}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1643,7 +2081,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>8</v>
@@ -1678,7 +2116,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1694,7 +2132,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1718,7 +2156,71 @@
         <v>7</v>
       </c>
       <c r="B11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
         <v>8</v>
+      </c>
+      <c r="B13" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1728,10 +2230,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5C73E4-F5F1-43AF-8CF5-DAD34D594BD5}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1745,15 +2247,15 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>120</v>
+      <c r="A2" s="5">
+        <v>95</v>
       </c>
       <c r="B2">
-        <v>120</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1766,10 +2268,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="B4">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1782,15 +2284,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="B6">
-        <v>120</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>130</v>
+      <c r="A7" s="5">
+        <v>60</v>
       </c>
       <c r="B7">
         <v>120</v>
@@ -1801,15 +2303,15 @@
         <v>120</v>
       </c>
       <c r="B8">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="B9">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1822,10 +2324,82 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
+        <v>80</v>
+      </c>
+      <c r="B11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>65</v>
+      </c>
+      <c r="B16">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>40</v>
+      </c>
+      <c r="B17">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>65</v>
+      </c>
+      <c r="B18">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>70</v>
+      </c>
+      <c r="B19">
         <v>120</v>
       </c>
-      <c r="B11">
-        <v>120</v>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>65</v>
+      </c>
+      <c r="B20">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1835,10 +2409,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD78A46-777D-46C0-8477-D558DF0BBFAB}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1937,6 +2511,78 @@
         <v>2500</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>3500</v>
+      </c>
+      <c r="B12">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1500</v>
+      </c>
+      <c r="B13">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1700</v>
+      </c>
+      <c r="B14">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1100</v>
+      </c>
+      <c r="B15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2100</v>
+      </c>
+      <c r="B16">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>3500</v>
+      </c>
+      <c r="B17">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2500</v>
+      </c>
+      <c r="B18">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>1200</v>
+      </c>
+      <c r="B19">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1000</v>
+      </c>
+      <c r="B20">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new attributes, hence updated ERD and Sample data.
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538300\Documents\691\gdp_group4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538306\Documents\Annie_Documents\691\44691-Module1-Badami4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8018EF67-F840-4E42-8FD6-469222E0ECD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327C9C5A-FDC0-4E3E-B528-F7F32DF759B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="7" xr2:uid="{090C377B-AC9E-4432-9958-B414BFE4C8F2}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{090C377B-AC9E-4432-9958-B414BFE4C8F2}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="139">
   <si>
     <t>user_id</t>
   </si>
@@ -439,6 +439,24 @@
   </si>
   <si>
     <t>push up dips</t>
+  </si>
+  <si>
+    <t>calories_date</t>
+  </si>
+  <si>
+    <t>oz_date</t>
+  </si>
+  <si>
+    <t>sleep_date</t>
+  </si>
+  <si>
+    <t>step_date</t>
+  </si>
+  <si>
+    <t>admin_password</t>
+  </si>
+  <si>
+    <t>user_password</t>
   </si>
 </sst>
 </file>
@@ -816,21 +834,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9072E92-96AB-4278-9757-75DAEE2DBEE6}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="2" max="3" width="25.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -838,515 +856,537 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>24</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>140</v>
       </c>
-      <c r="H2" s="4">
+      <c r="I2" s="4">
         <v>6.2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>500</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>8.1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>49</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>53</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>22</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>80</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>6.2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>91</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>53</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>28</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>90</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>5.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>90</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>53</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>10</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>50</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>40</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>24</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>42</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>170</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>6.1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>41</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>24</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>59</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>185</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>6.3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" t="s">
         <v>45</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>60</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>170</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>6.1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>51</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>24</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>40</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>180</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>5.1100000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" t="s">
         <v>47</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>52</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>53</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>38</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>120</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>5.8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" t="s">
         <v>85</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>87</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>24</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>45</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>158</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>6.4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" t="s">
         <v>92</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>95</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>53</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>33</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>138</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>27</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>159</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>5.3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" t="s">
         <v>96</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>97</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>24</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>41</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>169</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>5.5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" t="s">
         <v>98</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>99</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>53</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>17</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>130</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>5.2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" t="s">
         <v>100</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>101</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>53</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>22</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>141</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>103</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>24</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>43</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>176</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>5.7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" t="s">
         <v>43</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>104</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>24</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>20</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>110</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>5.3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" t="s">
         <v>106</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>105</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>53</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>23</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>159</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>5.4</v>
       </c>
     </row>
@@ -1378,22 +1418,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96344375-8305-4AE7-B026-B430EB9AB2D1}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1401,119 +1441,129 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1002</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1003</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1004</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1005</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1006</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1848,7 +1898,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2146,19 +2196,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94D898A-9782-46DE-A19A-69C6D87BB6B2}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.26953125" customWidth="1"/>
     <col min="2" max="2" width="23.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2168,8 +2219,11 @@
       <c r="C1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>10000</v>
       </c>
@@ -2180,7 +2234,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>12000</v>
       </c>
@@ -2191,7 +2245,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>15000</v>
       </c>
@@ -2202,7 +2256,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>20000</v>
       </c>
@@ -2213,7 +2267,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>13000</v>
       </c>
@@ -2224,7 +2278,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>14000</v>
       </c>
@@ -2235,7 +2289,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>15000</v>
       </c>
@@ -2246,7 +2300,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>17000</v>
       </c>
@@ -2257,7 +2311,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>18000</v>
       </c>
@@ -2268,7 +2322,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>15000</v>
       </c>
@@ -2279,7 +2333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10000</v>
       </c>
@@ -2290,7 +2344,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11000</v>
       </c>
@@ -2301,7 +2355,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>9000</v>
       </c>
@@ -2312,7 +2366,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>8000</v>
       </c>
@@ -2323,7 +2377,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>8000</v>
       </c>
@@ -2389,7 +2443,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2399,15 +2453,18 @@
     <col min="3" max="3" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>5</v>
       </c>
@@ -2415,7 +2472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>8</v>
       </c>
@@ -2423,7 +2480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>7</v>
       </c>
@@ -2431,7 +2488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>6</v>
       </c>
@@ -2439,7 +2496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>8</v>
       </c>
@@ -2447,7 +2504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2455,7 +2512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -2463,7 +2520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2471,7 +2528,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2479,7 +2536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -2487,7 +2544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -2495,7 +2552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -2503,7 +2560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -2511,7 +2568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>6</v>
       </c>
@@ -2519,7 +2576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>7</v>
       </c>
@@ -2566,10 +2623,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5C73E4-F5F1-43AF-8CF5-DAD34D594BD5}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A20"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2578,15 +2635,18 @@
     <col min="3" max="3" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>95</v>
       </c>
@@ -2594,7 +2654,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>100</v>
       </c>
@@ -2602,7 +2662,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>75</v>
       </c>
@@ -2610,7 +2670,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>90</v>
       </c>
@@ -2618,7 +2678,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>30</v>
       </c>
@@ -2626,7 +2686,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>60</v>
       </c>
@@ -2634,7 +2694,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>120</v>
       </c>
@@ -2642,7 +2702,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>90</v>
       </c>
@@ -2650,7 +2710,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>110</v>
       </c>
@@ -2658,7 +2718,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>80</v>
       </c>
@@ -2666,7 +2726,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>35</v>
       </c>
@@ -2674,7 +2734,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>50</v>
       </c>
@@ -2682,7 +2742,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>40</v>
       </c>
@@ -2690,7 +2750,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>55</v>
       </c>
@@ -2698,7 +2758,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>65</v>
       </c>
@@ -2745,10 +2805,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD78A46-777D-46C0-8477-D558DF0BBFAB}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2759,15 +2819,18 @@
     <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2000</v>
       </c>
@@ -2775,7 +2838,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1800</v>
       </c>
@@ -2783,7 +2846,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2200</v>
       </c>
@@ -2791,7 +2854,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2000</v>
       </c>
@@ -2799,7 +2862,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1900</v>
       </c>
@@ -2807,7 +2870,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2000</v>
       </c>
@@ -2815,7 +2878,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2500</v>
       </c>
@@ -2823,7 +2886,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2300</v>
       </c>
@@ -2831,7 +2894,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>2200</v>
       </c>
@@ -2839,7 +2902,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>3000</v>
       </c>
@@ -2847,7 +2910,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>3500</v>
       </c>
@@ -2855,7 +2918,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1500</v>
       </c>
@@ -2863,7 +2926,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1700</v>
       </c>
@@ -2871,7 +2934,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1100</v>
       </c>
@@ -2879,7 +2942,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2100</v>
       </c>

</xml_diff>

<commit_message>
Took new screenshots of the sample data.
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538306\Documents\Annie_Documents\691\44691-Module1-Badami4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0DF49D-F64E-4FD8-929E-41019868AC08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409B1E70-DF52-4A06-97C9-368323C440E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="1440" windowWidth="13700" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -467,7 +467,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,13 +483,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -505,7 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -523,6 +553,23 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -539,6 +586,1311 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF3724BF-7DD1-4358-9DE5-DCED270E5323}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2254250" y="3733800"/>
+          <a:ext cx="3479800" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Legend</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary Key</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Foreign Key</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Key, Foreign Key</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E558403F-F935-4346-94A8-BE40B47318A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1174750" y="1612900"/>
+          <a:ext cx="4089400" cy="831850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Legend</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Foreign Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Key, Foreign Key</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1327150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27CDD017-A832-4847-A044-FB6E00F5784A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2667000" y="2330450"/>
+          <a:ext cx="3067050" cy="831850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Legend</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Primary Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Foreign Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Key, Foreign Key</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{018FF6D5-929C-480D-89FF-D676E9F3A7CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4241800" y="508000"/>
+          <a:ext cx="2082800" cy="831850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Legend</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Foreign Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Key, Foreign Key</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1877283-9C2C-41D2-B344-B17D6EBECA9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4737100" y="647700"/>
+          <a:ext cx="2482850" cy="831850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Legend</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Foreign Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Key, Foreign Key</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A38BD31-6989-4C50-B609-A48621522E3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4241800" y="508000"/>
+          <a:ext cx="2082800" cy="831850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Legend</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Foreign Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Key, Foreign Key</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B54EC6F-C978-4B05-AF7D-DA6203E8B9E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4241800" y="508000"/>
+          <a:ext cx="2082800" cy="831850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Legend</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Foreign Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Key, Foreign Key</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A167674-386F-4D60-B446-936F6C6FFC7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3663950" y="508000"/>
+          <a:ext cx="2286000" cy="831850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Legend</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Foreign Key</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Key, Foreign Key</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -838,47 +2190,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.54296875" customWidth="1"/>
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1432,6 +2784,24 @@
       <c r="I20">
         <v>5.4</v>
       </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C22"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C23"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C24"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C25"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C26"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1456,43 +2826,45 @@
     <hyperlink ref="C19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="14.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="9.81640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1617,7 +2989,40 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C9" s="2"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1630,15 +3035,16 @@
     <hyperlink ref="B4" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1654,28 +3060,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1943,8 +3349,45 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.35">
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1953,7 +3396,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1965,16 +3408,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2246,6 +3689,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2254,28 +3699,28 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.26953125" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.6328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2367,7 +3812,7 @@
       <c r="D7" s="3">
         <v>44068</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -2382,7 +3827,7 @@
       <c r="D8" s="3">
         <v>44069</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -2397,7 +3842,7 @@
       <c r="D9" s="3">
         <v>44069</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -2412,7 +3857,7 @@
       <c r="D10" s="3">
         <v>44069</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -2427,7 +3872,7 @@
       <c r="D11" s="3">
         <v>44069</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -2442,7 +3887,7 @@
       <c r="D12" s="3">
         <v>44070</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -2559,6 +4004,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2567,7 +4013,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2578,18 +4024,18 @@
     <col min="4" max="4" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>43831</v>
       </c>
@@ -2600,7 +4046,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>44066</v>
       </c>
@@ -2610,8 +4056,9 @@
       <c r="C3" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>44066</v>
       </c>
@@ -2621,8 +4068,9 @@
       <c r="C4" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>44067</v>
       </c>
@@ -2632,8 +4080,9 @@
       <c r="C5" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>44068</v>
       </c>
@@ -2643,8 +4092,9 @@
       <c r="C6" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>44068</v>
       </c>
@@ -2654,8 +4104,9 @@
       <c r="C7" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>44069</v>
       </c>
@@ -2665,8 +4116,9 @@
       <c r="C8" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>44069</v>
       </c>
@@ -2677,7 +4129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>44069</v>
       </c>
@@ -2688,7 +4140,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>44069</v>
       </c>
@@ -2699,7 +4151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>44070</v>
       </c>
@@ -2710,7 +4162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>44071</v>
       </c>
@@ -2721,7 +4173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>44072</v>
       </c>
@@ -2732,7 +4184,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>44073</v>
       </c>
@@ -2743,7 +4195,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>44074</v>
       </c>
@@ -2800,6 +4252,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2808,24 +4261,25 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.36328125" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3040,6 +4494,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3047,27 +4502,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.90625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3282,5 +4737,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>